<commit_message>
modified:   README.md 	modified:   template_requirements_example.xlsx
</commit_message>
<xml_diff>
--- a/template_requirements_example.xlsx
+++ b/template_requirements_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/GitHub/Generate-testcases-and-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BE7784-9A2E-A64B-8395-18F734EED913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132F0D08-D702-7149-A38F-57396179E615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20100" xr2:uid="{611865A4-B98F-5341-9C6F-69FA41271498}"/>
   </bookViews>
@@ -37,21 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
-    <t>Requerimiento</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Id requerimiento</t>
-  </si>
-  <si>
-    <t>Consideraciones</t>
-  </si>
-  <si>
-    <t>Módulo</t>
-  </si>
-  <si>
     <t>Programación de horarios</t>
   </si>
   <si>
@@ -93,6 +78,21 @@
   </si>
   <si>
     <t>Gestión cuadro</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Requirement ID</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Considerations</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,101 +478,101 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1"/>
     </row>

</xml_diff>